<commit_message>
help function and git ignore adjustments
</commit_message>
<xml_diff>
--- a/Factorial-Analysis/Data/prova2.xlsx
+++ b/Factorial-Analysis/Data/prova2.xlsx
@@ -125,10 +125,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,7 +393,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>